<commit_message>
Errore de matriz distinto tamanioo
</commit_message>
<xml_diff>
--- a/RESULTADOS_Region_CASARES.xlsx
+++ b/RESULTADOS_Region_CASARES.xlsx
@@ -484,7 +484,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -570,7 +570,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -592,12 +592,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>280</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>255</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -638,7 +638,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>280.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -655,7 +655,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>255.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -706,7 +706,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>535.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -742,7 +742,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>170</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -759,7 +759,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>150</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>200</t>
         </is>
       </c>
     </row>
@@ -798,7 +798,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>250</t>
         </is>
       </c>
     </row>
@@ -810,12 +810,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>320</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>450</t>
         </is>
       </c>
     </row>
@@ -865,7 +865,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>28.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -897,7 +897,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -919,7 +919,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>37.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>39.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -973,12 +973,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>65.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>59.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>49.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>44.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>93.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>195.0</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>172.0</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>230.0</t>
         </is>
       </c>
     </row>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>287.0</t>
         </is>
       </c>
     </row>
@@ -1191,12 +1191,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>367.0</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>517.0</t>
         </is>
       </c>
     </row>
@@ -1214,7 +1214,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Cantidad de GEI en kg de CO2 Equivalente para el subsistema I-J: 2747.0</t>
+          <t>Cantidad de GEI en kg de CO2 Equivalente para el subsistema I-J: 0.0</t>
         </is>
       </c>
     </row>
@@ -1222,7 +1222,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Cantidad de GEI en kg de CO2 Equivalente para el subsistema J-K: 5328.0</t>
+          <t>Cantidad de GEI en kg de CO2 Equivalente para el subsistema J-K: 0.0</t>
         </is>
       </c>
     </row>
@@ -1230,7 +1230,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Cantidad de GEI en kg de CO2 Equivalente para el subsistema I-K: 0.0</t>
+          <t>Cantidad de GEI en kg de CO2 Equivalente para el subsistema I-K: 48473.0</t>
         </is>
       </c>
     </row>
@@ -1238,7 +1238,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Cantidad de GEI en kg de CO2 Equivalente para todo el sistema: 8075.0</t>
+          <t>Cantidad de GEI en kg de CO2 Equivalente para todo el sistema: 48473.0</t>
         </is>
       </c>
     </row>
@@ -1246,7 +1246,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Costo total de todo el sistema: [129110.]</t>
+          <t>Costo total de todo el sistema: [8381.]</t>
         </is>
       </c>
     </row>
@@ -1254,7 +1254,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Valor final de costo de inversión de ET: 30</t>
+          <t>Valor final de costo de inversión de ET: 4.657541095890411</t>
         </is>
       </c>
     </row>
@@ -1262,7 +1262,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Valor final de costo operativo de ET: 10</t>
+          <t>Valor final de costo operativo de ET: 691.43</t>
         </is>
       </c>
     </row>
@@ -1270,14 +1270,14 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Valor final de costo de inversión de CA: 90</t>
+          <t>Valor final de costo de inversión de CA: 7.934468955701832</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Valor final de costo operativo de CA: 135</t>
+          <t>Valor final de costo operativo de CA: 11.67591104634009</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Errores solucionados para matrices cuadradas
</commit_message>
<xml_diff>
--- a/RESULTADOS_Region_CASARES.xlsx
+++ b/RESULTADOS_Region_CASARES.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,11 +470,6 @@
           <t>J3</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>J4</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -497,11 +492,6 @@
           <t>0</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -524,11 +514,6 @@
           <t>0</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -551,16 +536,11 @@
           <t>0</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>I4</t>
+          <t>SUMA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -578,62 +558,57 @@
           <t>0</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>SUMA</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
+    </row>
+    <row r="9"/>
     <row r="10"/>
-    <row r="11"/>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>K1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>K2</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>K3</t>
+        </is>
+      </c>
+    </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>J1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>K1</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>K2</t>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>I1</t>
+          <t>J2</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -642,6 +617,11 @@
         </is>
       </c>
       <c r="C13" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -650,7 +630,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>I2</t>
+          <t>J3</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -659,6 +639,11 @@
         </is>
       </c>
       <c r="C14" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -667,7 +652,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>I3</t>
+          <t>SUMA</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -680,72 +665,97 @@
           <t>0.0</t>
         </is>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>I4</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>SUMA</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="18"/>
-    <row r="19"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>K1</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>K2</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>K3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>I1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>I2</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>K1</t>
+          <t>200</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>K2</t>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>I1</t>
+          <t>I3</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -754,68 +764,31 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>I2</t>
+          <t>SUMA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>350</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>I3</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
           <t>200</t>
         </is>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>I4</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
-      </c>
-    </row>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="23"/>
+    <row r="24"/>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SUMA</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>320</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>450</t>
+          <t>Distribución de camiones en todo el sistema</t>
         </is>
       </c>
     </row>
@@ -824,43 +797,95 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Distribución de camiones en todo el sistema</t>
-        </is>
-      </c>
-    </row>
-    <row r="29"/>
-    <row r="30"/>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>J1</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>J2</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>J3</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>I1</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>I2</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>I3</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>J1</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>J2</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>J3</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>J4</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>I1</t>
+          <t>SUMA</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -878,97 +903,35 @@
           <t>0.0</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>I2</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>I3</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
+    </row>
+    <row r="33"/>
+    <row r="34"/>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>I4</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>K1</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>K2</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>0.0</t>
+          <t>K3</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>SUMA</t>
+          <t>J1</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -986,94 +949,114 @@
           <t>0.0</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="37"/>
-    <row r="38"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>J2</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>J3</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>SUMA</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>K1</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>K2</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>J1</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>J2</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="40"/>
+    <row r="41"/>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>J3</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>K1</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>K2</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>K3</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>J4</t>
+          <t>I1</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>35.0</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1082,139 +1065,108 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>I2</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>69.0</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>I3</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>46.0</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>SUMA</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>K1</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>K2</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>I1</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>195.0</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>104.0</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>46.0</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="47"/>
+    <row r="48"/>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>I2</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>172.0</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>I3</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>230.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>I4</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>287.0</t>
-        </is>
-      </c>
-    </row>
+          <t>Distribución de Gases de Efecto Invernadero en todo el sistema</t>
+        </is>
+      </c>
+    </row>
+    <row r="50"/>
+    <row r="51"/>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>SUMA</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>367.0</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>517.0</t>
+          <t>Cantidad de GEI en kg de CO2 Equivalente para el subsistema I-J: 0.0</t>
         </is>
       </c>
     </row>
     <row r="53"/>
-    <row r="54"/>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Distribución de Gases de Efecto Invernadero en todo el sistema</t>
-        </is>
-      </c>
-    </row>
-    <row r="56"/>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Cantidad de GEI en kg de CO2 Equivalente para el subsistema J-K: 0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="55"/>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Cantidad de GEI en kg de CO2 Equivalente para el subsistema I-K: 11450.0</t>
+        </is>
+      </c>
+    </row>
     <row r="57"/>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Cantidad de GEI en kg de CO2 Equivalente para el subsistema I-J: 0.0</t>
+          <t>Cantidad de GEI en kg de CO2 Equivalente para todo el sistema: 11450.0</t>
         </is>
       </c>
     </row>
@@ -1222,7 +1174,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Cantidad de GEI en kg de CO2 Equivalente para el subsistema J-K: 0.0</t>
+          <t>Costo total de todo el sistema: [46604.]</t>
         </is>
       </c>
     </row>
@@ -1230,7 +1182,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Cantidad de GEI en kg de CO2 Equivalente para el subsistema I-K: 48473.0</t>
+          <t>Valor final de costo de inversión de ET: 4.657541095890411</t>
         </is>
       </c>
     </row>
@@ -1238,7 +1190,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Cantidad de GEI en kg de CO2 Equivalente para todo el sistema: 48473.0</t>
+          <t>Valor final de costo operativo de ET: 691.43</t>
         </is>
       </c>
     </row>
@@ -1246,38 +1198,14 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Costo total de todo el sistema: [8381.]</t>
-        </is>
-      </c>
-    </row>
-    <row r="67"/>
+          <t>Valor final de costo de inversión de CA: 9.215379825653798</t>
+        </is>
+      </c>
+    </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Valor final de costo de inversión de ET: 4.657541095890411</t>
-        </is>
-      </c>
-    </row>
-    <row r="69"/>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Valor final de costo operativo de ET: 691.43</t>
-        </is>
-      </c>
-    </row>
-    <row r="71"/>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Valor final de costo de inversión de CA: 7.934468955701832</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Valor final de costo operativo de CA: 11.67591104634009</t>
+          <t>Valor final de costo operativo de CA: 15.620377613753833</t>
         </is>
       </c>
     </row>

</xml_diff>